<commit_message>
updated MC (tracks activity + capacity by year) + plotting with boxplots
</commit_message>
<xml_diff>
--- a/examples/puerto_rico/data/scenarios.xlsx
+++ b/examples/puerto_rico/data/scenarios.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="49">
   <si>
     <t>Scenario</t>
   </si>
@@ -78,15 +78,6 @@
     <t>EC_BIO</t>
   </si>
   <si>
-    <t>EC_COAL</t>
-  </si>
-  <si>
-    <t>EC_DSL_CC</t>
-  </si>
-  <si>
-    <t>EC_OIL</t>
-  </si>
-  <si>
     <t>EC_NG_CC</t>
   </si>
   <si>
@@ -114,12 +105,6 @@
     <t>ED_WIND</t>
   </si>
   <si>
-    <t>EI_BATT</t>
-  </si>
-  <si>
-    <t>EI_SOLPV</t>
-  </si>
-  <si>
     <t>include_baseload</t>
   </si>
   <si>
@@ -181,6 +166,9 @@
   </si>
   <si>
     <t>MinGrowthSeed</t>
+  </si>
+  <si>
+    <t>ED_NG_CC</t>
   </si>
 </sst>
 </file>
@@ -502,7 +490,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,92 +517,92 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -631,7 +619,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>1000</v>
@@ -654,10 +642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,16 +675,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -704,16 +692,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -721,16 +709,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -738,16 +726,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -755,16 +743,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -772,16 +760,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -789,16 +777,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -806,16 +794,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,16 +811,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -840,16 +828,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -857,16 +845,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -874,161 +862,118 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
+      <c r="C14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" t="s">
-        <v>36</v>
+      <c r="C18" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
-        <v>36</v>
+      <c r="D19" t="s">
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1037,7 +982,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,152 +1009,149 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1249,53 +1191,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>